<commit_message>
He quitado la valencia de -2 al oxígeno
</commit_message>
<xml_diff>
--- a/public/Hojas de Calculo/ElementosSinFormulas.xlsx
+++ b/public/Hojas de Calculo/ElementosSinFormulas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t xml:space="preserve">z</t>
   </si>
@@ -305,9 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,-2</t>
   </si>
   <si>
     <t xml:space="preserve">Paladio</t>
@@ -601,19 +598,19 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
-      <selection pane="bottomRight" activeCell="F73" activeCellId="0" sqref="F73"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1459,8 +1456,8 @@
       <c r="C33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>93</v>
+      <c r="D33" s="0" t="n">
+        <v>-2</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>37</v>
@@ -1480,10 +1477,10 @@
         <v>46</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>59</v>
@@ -1506,10 +1503,10 @@
         <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>1</v>
@@ -1532,10 +1529,10 @@
         <v>78</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>59</v>
@@ -1558,10 +1555,10 @@
         <v>82</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>59</v>
@@ -1584,10 +1581,10 @@
         <v>19</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D38" s="4" t="n">
         <v>1</v>
@@ -1610,10 +1607,10 @@
         <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D39" s="4" t="n">
         <v>2</v>
@@ -1636,10 +1633,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>1</v>
@@ -1662,13 +1659,13 @@
         <v>34</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>1</v>
@@ -1688,13 +1685,13 @@
         <v>14</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>1</v>
@@ -1714,10 +1711,10 @@
         <v>11</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D43" s="4" t="n">
         <v>1</v>
@@ -1740,13 +1737,13 @@
         <v>22</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>1</v>
@@ -1766,10 +1763,10 @@
         <v>53</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>47</v>
@@ -1791,7 +1788,7 @@
   <autoFilter ref="A1:H87"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1811,7 +1808,7 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -1879,13 +1876,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>